<commit_message>
Add: BC\DQN\PPO for Tielie-case
</commit_message>
<xml_diff>
--- a/gym_SelfHealing/selfhealing_env/envs/case_data/Case_33BW_Data.xlsx
+++ b/gym_SelfHealing/selfhealing_env/envs/case_data/Case_33BW_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Academic\SelfHealing\gym_pds\envs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Academic\SelfHealing\gym_SelfHealing\selfhealing_env\envs\case_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B0D8AD-37C7-4F0D-9AE4-43A9ECD2A280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D3E7DA-B53F-4A86-BEDD-E64BD01FEA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="1425" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9060" yWindow="1425" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="17" r:id="rId1"/>
@@ -527,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A5520F-0884-4749-AEAB-24535D6EEF87}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BC601C-6925-4DEF-89B0-5C277128F18A}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>